<commit_message>
Proyecto de nuevas planillas
</commit_message>
<xml_diff>
--- a/LISTA DE ROPA ESTACIONES.xlsx
+++ b/LISTA DE ROPA ESTACIONES.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzo_\Desktop\Olivos_Combustibles_SRL\Olivos_Combustibles_SRL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OSCAR\Desktop\Olivos_Combustibles_SRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471C77E8-FD56-4D6C-A03A-0E8E1EB42E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5F4E0370-5AF5-415F-A720-300AAEE97B62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>TALLE</t>
   </si>
@@ -88,13 +87,22 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AXION OLIVOS - Mariano Pelliza 3892 - </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +120,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,10 +188,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,8 +212,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,19 +532,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F30B70-C9B3-43F7-8625-321801AFF180}">
-  <dimension ref="B4:E49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="60.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -534,7 +559,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -547,8 +572,14 @@
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7">
+        <v>712880</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>6301</v>
       </c>
@@ -562,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6301</v>
       </c>
@@ -576,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6130</v>
       </c>
@@ -590,7 +621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6130</v>
       </c>
@@ -604,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6517</v>
       </c>
@@ -618,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>6502</v>
       </c>
@@ -632,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>3304</v>
       </c>
@@ -646,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>6701</v>
       </c>
@@ -658,25 +689,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
@@ -684,7 +715,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
@@ -697,8 +728,14 @@
       <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="7">
+        <v>92400</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>3102</v>
       </c>
@@ -712,7 +749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3102</v>
       </c>
@@ -726,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>3102</v>
       </c>
@@ -740,55 +777,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>12</v>
       </c>
@@ -796,7 +833,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,8 +846,14 @@
       <c r="E38" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="7">
+        <v>278600</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>9300</v>
       </c>
@@ -824,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>9300</v>
       </c>
@@ -838,59 +881,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F53" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1083880</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>